<commit_message>
Create second version of roll control in hover with a Simulink model and execution code.
</commit_message>
<xml_diff>
--- a/parameters/catiaMeas.xlsx
+++ b/parameters/catiaMeas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomo\TomoCode\aae451\aae451-senior-design\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C55840A-7136-4845-878D-688DADF1F696}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153CA52F-6150-4755-9C9D-1B70428E6677}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WingsForward1m" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
   <si>
     <t xml:space="preserve">Component         </t>
   </si>
@@ -525,13 +525,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1008,11 +1013,6 @@
       </c>
       <c r="Q9">
         <v>-0.255</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1027,15 +1027,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>-6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>-8.5000000000000006E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1510,11 +1510,6 @@
       </c>
       <c r="Q9">
         <v>-0.255</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R12" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>